<commit_message>
Update journal de travail
</commit_message>
<xml_diff>
--- a/Documentation/Journal_De_Travail.xlsx
+++ b/Documentation/Journal_De_Travail.xlsx
@@ -585,7 +585,7 @@
   <dimension ref="A1:H734"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="M40" sqref="M40"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="51.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1566,9 +1566,12 @@
       <c r="B42" s="4">
         <v>0.33819444444444446</v>
       </c>
+      <c r="C42" s="4">
+        <v>0.36041666666666666</v>
+      </c>
       <c r="D42" s="4">
         <f t="shared" si="0"/>
-        <v>-0.33819444444444446</v>
+        <v>2.2222222222222199E-2</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>11</v>
@@ -1581,9 +1584,15 @@
       </c>
     </row>
     <row r="43" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>45014</v>
+      </c>
+      <c r="B43" s="4">
+        <v>0.59861111111111109</v>
+      </c>
       <c r="D43" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.59861111111111109</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>